<commit_message>
Model class ları oluşturuldu.
</commit_message>
<xml_diff>
--- a/ShoppingCart.UI/App_Data/schema.xlsx
+++ b/ShoppingCart.UI/App_Data/schema.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CA4265-489C-4083-A3DD-130B49226B62}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,8 +18,90 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="H4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Kampanyanın uygulanacağı kategori id değeri.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Kampanyanın geçerli olması için, aynı kategoriden alınan minimum ürün adedi.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Kupon indiriminin geçerli olması için minimum alışveriş tutarı.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Product</t>
   </si>
@@ -61,14 +142,23 @@
     <t>Coupon</t>
   </si>
   <si>
-    <t>MinPrice</t>
+    <t>MinimumItem</t>
+  </si>
+  <si>
+    <t>DiscountPercent</t>
+  </si>
+  <si>
+    <t>MinimumPrice</t>
+  </si>
+  <si>
+    <t>Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +174,19 @@
       <family val="2"/>
       <charset val="162"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -158,13 +261,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,29 +548,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="1.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="1.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="1.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="1.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -494,19 +599,22 @@
       <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="I3" s="2"/>
       <c r="J3" s="4" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>2</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
@@ -518,27 +626,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>3</v>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>8</v>
+      <c r="G5" s="2"/>
+      <c r="H5" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>